<commit_message>
updates, new plots, redid pam stats
</commit_message>
<xml_diff>
--- a/Stats_results_phytoclass.xlsx
+++ b/Stats_results_phytoclass.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cathe\Dropbox\PC\Desktop\MS Thesis\MS_Thesis_2023-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7931A926-386A-48AF-90C9-F55C359DEFF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434C6EB8-BBB4-45C4-8CF8-1291754E3719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2C8FDCF4-0945-415E-9590-0F187949B922}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="MANOVAs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1068,7 +1067,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
pushing everything just in case
</commit_message>
<xml_diff>
--- a/Stats_results_phytoclass.xlsx
+++ b/Stats_results_phytoclass.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cathe\Dropbox\PC\Desktop\MS Thesis\MS_Thesis_2023-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434C6EB8-BBB4-45C4-8CF8-1291754E3719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFD357B-58A7-4C1B-8A31-25D61BA4A892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2C8FDCF4-0945-415E-9590-0F187949B922}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2C8FDCF4-0945-415E-9590-0F187949B922}"/>
   </bookViews>
   <sheets>
     <sheet name="ANOVAs - percent dif" sheetId="1" r:id="rId1"/>
@@ -384,7 +384,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,6 +403,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -416,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -454,6 +466,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -771,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A17F176-753C-47BC-A81F-3418BBE24096}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -844,13 +862,13 @@
       <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -882,7 +900,7 @@
       <c r="I3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="14" t="s">
         <v>31</v>
       </c>
     </row>
@@ -914,7 +932,7 @@
       <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="14" t="s">
         <v>34</v>
       </c>
     </row>
@@ -946,7 +964,7 @@
       <c r="I5" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="14" t="s">
         <v>42</v>
       </c>
     </row>
@@ -978,7 +996,7 @@
       <c r="I6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="14" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1010,7 +1028,7 @@
       <c r="I7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="14" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1042,7 +1060,7 @@
       <c r="I8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="14" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1066,7 +1084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{702E5FEC-7A42-4666-9134-1B29BDF2CD23}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
new figures plus normality tests and RBC anovas
</commit_message>
<xml_diff>
--- a/Stats_results_phytoclass.xlsx
+++ b/Stats_results_phytoclass.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cathe\Dropbox\PC\Desktop\MS Thesis\MS_Thesis_2023-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322CB026-1D1D-4759-B945-D27C30240D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DF75A4-47A4-42C1-9D8A-CEA79D563FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="1" activeTab="1" xr2:uid="{2C8FDCF4-0945-415E-9590-0F187949B922}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="1" activeTab="1" xr2:uid="{2C8FDCF4-0945-415E-9590-0F187949B922}"/>
   </bookViews>
   <sheets>
     <sheet name="ANOVAs - percent dif" sheetId="1" r:id="rId1"/>
-    <sheet name="ANOVAs - biomass by bioassay" sheetId="3" r:id="rId2"/>
-    <sheet name="MANOVAs" sheetId="2" r:id="rId3"/>
+    <sheet name="RCB ANOVAs - biomass" sheetId="4" r:id="rId2"/>
+    <sheet name="ANOVAs - biomass by bioassay" sheetId="3" r:id="rId3"/>
+    <sheet name="MANOVAs" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,8 +63,175 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Catherine Schlenker</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{680926B3-4EF8-48D1-BD75-1E9C089DBA4E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Catherine Schlenker:
+Independent variable for all = Treatment group</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{5A25EBA7-83F9-4DB7-8CA8-E0252739FFD7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Catherine Schlenker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+using interaction between treatment and bioassay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{E198D16F-0D5A-4FB1-BBA7-302CADE3CA8C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Catherine Schlenker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+using interaction between treatment and bioassay THIS IS FROM R</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{BB155CE0-625D-4023-AD23-4FD0C3D02EB4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Catherine Schlenker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+using interaction between treatment and bioassay SPSS</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{B9F65478-D03E-459F-9CA6-7A32D119CB7A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Catherine Schlenker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+using interaction between treatment and bioassay SPSS
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{2DA4353C-DA3D-44AC-BCC0-A9038E4C7B94}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Catherine Schlenker:
+Independent variable for all = Treatment group</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{7D1EBCDE-49C8-48B4-BF7D-6E9BC0D44771}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Catherine Schlenker:
+Independent variable for all = Treatment group</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A28" authorId="0" shapeId="0" xr:uid="{56CCD6C1-B988-457A-8624-39CD3F649224}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Catherine Schlenker:
+Independent variable for all = Treatment group</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="157">
   <si>
     <t>Dependent variable (% change from control)</t>
   </si>
@@ -589,6 +757,54 @@
   <si>
     <t>control dif from everything all &lt; 0.0001 except hp p = 0.0102 and lp p = 0.0001, din different from everything p &lt; 0.0001 except din+hp p = 0.0281 din+lp p = 0.0413, din+hp-hp, lp, t0 p &lt; 0.0001; din+lp-hp, lp, t0 p &lt; 0.0001; hp-t0 p = 0.0004, lp-t0 p = 0.0369</t>
   </si>
+  <si>
+    <t>RCB ANOVA</t>
+  </si>
+  <si>
+    <t>Dependent variable (biomass)</t>
+  </si>
+  <si>
+    <t>df treatment</t>
+  </si>
+  <si>
+    <t>df bioassay</t>
+  </si>
+  <si>
+    <t>f treatment</t>
+  </si>
+  <si>
+    <t>f bioassay</t>
+  </si>
+  <si>
+    <t>p treatment</t>
+  </si>
+  <si>
+    <t>p bioassay</t>
+  </si>
+  <si>
+    <t>&lt; 2e-16</t>
+  </si>
+  <si>
+    <t>Dependent variable (percent change)</t>
+  </si>
+  <si>
+    <t>Dependent variable (ln(biomass))</t>
+  </si>
+  <si>
+    <t>Dependent variable (ln(percent change))</t>
+  </si>
+  <si>
+    <t>Levene's test F</t>
+  </si>
+  <si>
+    <t>Levene's test p</t>
+  </si>
+  <si>
+    <t>&lt;0.001</t>
+  </si>
+  <si>
+    <t>DF Levene;s</t>
+  </si>
 </sst>
 </file>
 
@@ -597,7 +813,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -642,6 +858,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -700,7 +922,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -746,9 +968,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -758,6 +977,19 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,9 +1008,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -816,7 +1048,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -922,7 +1154,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1064,7 +1296,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1075,7 +1307,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1366,14 +1598,1015 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12773B5D-97E8-4039-B93C-89E44230DCC5}">
+  <dimension ref="A1:M1048576"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D26" sqref="D26:G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="39" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="26"/>
+    <col min="9" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="26"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J1" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1" t="s">
+        <v>153</v>
+      </c>
+      <c r="M1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>113.92</v>
+      </c>
+      <c r="E2">
+        <v>24.02</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" s="25">
+        <v>1.9699999999999999E-12</v>
+      </c>
+      <c r="H2" s="30">
+        <v>27</v>
+      </c>
+      <c r="I2">
+        <v>2.7126000000000001</v>
+      </c>
+      <c r="J2" s="27">
+        <v>1.3239999999999999E-4</v>
+      </c>
+      <c r="K2" s="29">
+        <v>27</v>
+      </c>
+      <c r="L2">
+        <v>7.4809999999999999</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" s="32">
+        <v>3.903</v>
+      </c>
+      <c r="E3" s="32">
+        <v>93.069000000000003</v>
+      </c>
+      <c r="F3" s="33">
+        <v>1.2899999999999999E-3</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="H3" s="30">
+        <v>27</v>
+      </c>
+      <c r="I3">
+        <v>2.3639000000000001</v>
+      </c>
+      <c r="J3" s="16">
+        <v>9.0390000000000002E-4</v>
+      </c>
+      <c r="K3" s="29">
+        <v>27</v>
+      </c>
+      <c r="L3">
+        <v>4.5970000000000004</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="32">
+        <v>23.21</v>
+      </c>
+      <c r="E4" s="32">
+        <v>14.18</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="G4" s="34">
+        <v>4.7199999999999999E-8</v>
+      </c>
+      <c r="H4" s="30">
+        <v>27</v>
+      </c>
+      <c r="I4">
+        <v>3.2056</v>
+      </c>
+      <c r="J4" s="31">
+        <v>8.6130000000000004E-6</v>
+      </c>
+      <c r="K4" s="29">
+        <v>27</v>
+      </c>
+      <c r="L4">
+        <v>22.89</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" s="32">
+        <v>88.35</v>
+      </c>
+      <c r="E5" s="32">
+        <v>19.68</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" s="34">
+        <v>1.4000000000000001E-10</v>
+      </c>
+      <c r="H5" s="30">
+        <v>27</v>
+      </c>
+      <c r="I5">
+        <v>3.0459000000000001</v>
+      </c>
+      <c r="J5" s="31">
+        <v>2.0849999999999999E-5</v>
+      </c>
+      <c r="K5" s="29">
+        <v>27</v>
+      </c>
+      <c r="L5">
+        <v>6.5579999999999998</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>119.43</v>
+      </c>
+      <c r="E6">
+        <v>24.23</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" s="25">
+        <v>1.61E-12</v>
+      </c>
+      <c r="H6" s="30">
+        <v>27</v>
+      </c>
+      <c r="I6">
+        <v>2.4906999999999999</v>
+      </c>
+      <c r="J6" s="16">
+        <v>4.5130000000000002E-4</v>
+      </c>
+      <c r="K6" s="29">
+        <v>27</v>
+      </c>
+      <c r="L6">
+        <v>6.391</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" s="32">
+        <v>16.350000000000001</v>
+      </c>
+      <c r="E7" s="32">
+        <v>13.32</v>
+      </c>
+      <c r="F7" s="34">
+        <v>5.7199999999999999E-14</v>
+      </c>
+      <c r="G7" s="34">
+        <v>1.24E-7</v>
+      </c>
+      <c r="H7" s="30">
+        <v>27</v>
+      </c>
+      <c r="I7">
+        <v>1.0891999999999999</v>
+      </c>
+      <c r="J7" s="24">
+        <v>0.36509999999999998</v>
+      </c>
+      <c r="K7" s="29">
+        <v>27</v>
+      </c>
+      <c r="L7">
+        <v>5.2960000000000003</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>6.3739999999999997</v>
+      </c>
+      <c r="E8" s="32">
+        <v>11.356</v>
+      </c>
+      <c r="F8" s="25">
+        <v>6.6499999999999999E-6</v>
+      </c>
+      <c r="G8" s="25">
+        <v>1.15E-6</v>
+      </c>
+      <c r="H8" s="30">
+        <v>27</v>
+      </c>
+      <c r="I8">
+        <v>2.5545</v>
+      </c>
+      <c r="J8" s="16">
+        <v>3.1750000000000002E-4</v>
+      </c>
+      <c r="K8" s="29">
+        <v>27</v>
+      </c>
+      <c r="L8">
+        <v>3.2170000000000001</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>9.7650000000000006</v>
+      </c>
+      <c r="E11">
+        <v>3.355</v>
+      </c>
+      <c r="F11" s="24">
+        <v>9.4200000000000002E-4</v>
+      </c>
+      <c r="G11" s="23">
+        <v>5.5320000000000001E-2</v>
+      </c>
+      <c r="H11" s="28"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>0.373</v>
+      </c>
+      <c r="E12">
+        <v>19.452000000000002</v>
+      </c>
+      <c r="F12">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="G12" s="25">
+        <v>6.6699999999999995E-5</v>
+      </c>
+      <c r="H12" s="28"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>4.0810000000000004</v>
+      </c>
+      <c r="E13">
+        <v>4.4340000000000002</v>
+      </c>
+      <c r="F13" s="24">
+        <v>2.58E-2</v>
+      </c>
+      <c r="G13" s="24">
+        <v>2.5700000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>7.468</v>
+      </c>
+      <c r="E14">
+        <v>5.8280000000000003</v>
+      </c>
+      <c r="F14" s="24">
+        <v>2.9299999999999999E-3</v>
+      </c>
+      <c r="G14" s="24">
+        <v>1.0749999999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>5.1920000000000002</v>
+      </c>
+      <c r="E15">
+        <v>4.8220000000000001</v>
+      </c>
+      <c r="F15" s="24">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="G15" s="24">
+        <v>1.9900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>1.548</v>
+      </c>
+      <c r="E16">
+        <v>6.5970000000000004</v>
+      </c>
+      <c r="F16" s="26">
+        <v>0.25048999999999999</v>
+      </c>
+      <c r="G16" s="24">
+        <v>6.9699999999999996E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="E17">
+        <v>3.6640000000000001</v>
+      </c>
+      <c r="F17" s="26">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="G17" s="24">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="C19" t="s">
+        <v>144</v>
+      </c>
+      <c r="D19" t="s">
+        <v>145</v>
+      </c>
+      <c r="E19" t="s">
+        <v>146</v>
+      </c>
+      <c r="F19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>321.35000000000002</v>
+      </c>
+      <c r="E20">
+        <v>61.47</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="H20" s="30">
+        <v>27</v>
+      </c>
+      <c r="I20">
+        <v>1.2904</v>
+      </c>
+      <c r="J20" s="24">
+        <v>0.1787</v>
+      </c>
+      <c r="K20" s="29">
+        <v>27</v>
+      </c>
+      <c r="L20">
+        <v>5.2130000000000001</v>
+      </c>
+      <c r="M20" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21" s="32">
+        <v>3.79</v>
+      </c>
+      <c r="E21" s="32">
+        <v>105.33</v>
+      </c>
+      <c r="F21" s="33">
+        <v>1.64E-3</v>
+      </c>
+      <c r="G21" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="H21" s="30">
+        <v>27</v>
+      </c>
+      <c r="I21">
+        <v>2.5489999999999999</v>
+      </c>
+      <c r="J21" s="16">
+        <v>5.3689999999999999E-4</v>
+      </c>
+      <c r="K21" s="29">
+        <v>27</v>
+      </c>
+      <c r="L21">
+        <v>5.1980000000000004</v>
+      </c>
+      <c r="M21" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" s="32">
+        <v>34.692</v>
+      </c>
+      <c r="E22" s="32">
+        <v>8.9459999999999997</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="G22" s="34">
+        <v>1.9700000000000001E-5</v>
+      </c>
+      <c r="H22" s="30">
+        <v>27</v>
+      </c>
+      <c r="I22">
+        <v>2.2086999999999999</v>
+      </c>
+      <c r="J22" s="16">
+        <v>2.0969999999999999E-3</v>
+      </c>
+      <c r="K22" s="29">
+        <v>27</v>
+      </c>
+      <c r="L22">
+        <v>19.571000000000002</v>
+      </c>
+      <c r="M22" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23" s="32">
+        <v>123.66</v>
+      </c>
+      <c r="E23" s="32">
+        <v>18.670000000000002</v>
+      </c>
+      <c r="F23" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="G23" s="34">
+        <v>3.9399999999999998E-10</v>
+      </c>
+      <c r="H23" s="30">
+        <v>27</v>
+      </c>
+      <c r="I23">
+        <v>2.1597</v>
+      </c>
+      <c r="J23" s="16">
+        <v>2.7269999999999998E-3</v>
+      </c>
+      <c r="K23" s="29">
+        <v>27</v>
+      </c>
+      <c r="L23">
+        <v>6.2350000000000003</v>
+      </c>
+      <c r="M23" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" s="32">
+        <v>168.25</v>
+      </c>
+      <c r="E24" s="32">
+        <v>43.75</v>
+      </c>
+      <c r="F24" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="H24" s="30">
+        <v>27</v>
+      </c>
+      <c r="I24">
+        <v>2.1804000000000001</v>
+      </c>
+      <c r="J24" s="16">
+        <v>2.441E-3</v>
+      </c>
+      <c r="K24" s="29">
+        <v>27</v>
+      </c>
+      <c r="L24">
+        <v>8.5640000000000001</v>
+      </c>
+      <c r="M24" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25" s="32">
+        <v>16.260000000000002</v>
+      </c>
+      <c r="E25" s="32">
+        <v>13.48</v>
+      </c>
+      <c r="F25" s="34">
+        <v>6.6499999999999994E-14</v>
+      </c>
+      <c r="G25" s="34">
+        <v>1.03E-7</v>
+      </c>
+      <c r="H25" s="30">
+        <v>27</v>
+      </c>
+      <c r="I25">
+        <v>10.050800000000001</v>
+      </c>
+      <c r="J25" s="24">
+        <v>0.4108</v>
+      </c>
+      <c r="K25" s="29">
+        <v>27</v>
+      </c>
+      <c r="L25">
+        <v>4.6719999999999997</v>
+      </c>
+      <c r="M25" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26" s="32">
+        <v>9.9649999999999999</v>
+      </c>
+      <c r="E26" s="32">
+        <v>11.576000000000001</v>
+      </c>
+      <c r="F26" s="34">
+        <v>4.8799999999999997E-9</v>
+      </c>
+      <c r="G26" s="34">
+        <v>8.9400000000000004E-7</v>
+      </c>
+      <c r="H26" s="30">
+        <v>27</v>
+      </c>
+      <c r="I26">
+        <v>2.5865999999999998</v>
+      </c>
+      <c r="J26" s="16">
+        <v>2.6589999999999999E-3</v>
+      </c>
+      <c r="K26" s="29">
+        <v>27</v>
+      </c>
+      <c r="L26">
+        <v>2.6989999999999998</v>
+      </c>
+      <c r="M26" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>9.7650000000000006</v>
+      </c>
+      <c r="E29">
+        <v>3.355</v>
+      </c>
+      <c r="F29" s="24">
+        <v>9.4200000000000002E-4</v>
+      </c>
+      <c r="G29" s="23">
+        <v>5.5320000000000001E-2</v>
+      </c>
+      <c r="H29" s="28"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>0.373</v>
+      </c>
+      <c r="E30">
+        <v>19.452000000000002</v>
+      </c>
+      <c r="F30">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="G30" s="25">
+        <v>6.6699999999999995E-5</v>
+      </c>
+      <c r="H30" s="28"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>4.0810000000000004</v>
+      </c>
+      <c r="E31">
+        <v>4.4340000000000002</v>
+      </c>
+      <c r="F31" s="24">
+        <v>2.58E-2</v>
+      </c>
+      <c r="G31" s="24">
+        <v>2.5700000000000001E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>7.468</v>
+      </c>
+      <c r="E32">
+        <v>5.8280000000000003</v>
+      </c>
+      <c r="F32" s="24">
+        <v>2.9299999999999999E-3</v>
+      </c>
+      <c r="G32" s="24">
+        <v>1.0749999999999999E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33">
+        <v>5.1920000000000002</v>
+      </c>
+      <c r="E33">
+        <v>4.8220000000000001</v>
+      </c>
+      <c r="F33" s="24">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="G33" s="24">
+        <v>1.9900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>1.548</v>
+      </c>
+      <c r="E34">
+        <v>6.5970000000000004</v>
+      </c>
+      <c r="F34" s="26">
+        <v>0.25048999999999999</v>
+      </c>
+      <c r="G34" s="24">
+        <v>6.9699999999999996E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="E35">
+        <v>3.6640000000000001</v>
+      </c>
+      <c r="F35" s="26">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="G35" s="24">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="1048576" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M1048576" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02F6CD7-2B91-414A-B381-AE1014A5E445}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="H8" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1384,9 +2617,10 @@
     <col min="6" max="7" width="15.5546875" customWidth="1"/>
     <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="13" max="13" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>92</v>
       </c>
@@ -1417,8 +2651,11 @@
       <c r="K1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -1437,19 +2674,19 @@
       <c r="F2" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-    </row>
-    <row r="3" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+    </row>
+    <row r="3" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -1462,21 +2699,21 @@
       <c r="D3" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="19" t="s">
         <v>132</v>
       </c>
       <c r="F3" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="22" t="s">
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-    </row>
-    <row r="4" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+    </row>
+    <row r="4" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -1492,22 +2729,22 @@
       <c r="E4" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-    </row>
-    <row r="5" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+    </row>
+    <row r="5" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -1520,21 +2757,21 @@
       <c r="D5" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18" t="s">
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-    </row>
-    <row r="6" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+    </row>
+    <row r="6" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -1550,22 +2787,22 @@
       <c r="E6" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-    </row>
-    <row r="7" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+    </row>
+    <row r="7" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>89</v>
       </c>
@@ -1578,21 +2815,21 @@
       <c r="D7" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18" t="s">
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-    </row>
-    <row r="8" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+    </row>
+    <row r="8" spans="1:13" ht="144" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -1602,28 +2839,28 @@
       <c r="C8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="18" t="s">
         <v>118</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-    </row>
-    <row r="9" spans="1:11" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+    </row>
+    <row r="9" spans="1:13" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>91</v>
       </c>
@@ -1636,26 +2873,26 @@
       <c r="D9" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18" t="s">
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{702E5FEC-7A42-4666-9134-1B29BDF2CD23}">
   <dimension ref="A1:I3"/>
   <sheetViews>

</xml_diff>

<commit_message>
permanova anosim and new figures
</commit_message>
<xml_diff>
--- a/Stats_results_phytoclass.xlsx
+++ b/Stats_results_phytoclass.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cathe\Dropbox\PC\Desktop\MS Thesis\MS_Thesis_2023-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DF75A4-47A4-42C1-9D8A-CEA79D563FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBA51BA-7E2B-4551-89E8-313C830C232F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="1" activeTab="1" xr2:uid="{2C8FDCF4-0945-415E-9590-0F187949B922}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2C8FDCF4-0945-415E-9590-0F187949B922}"/>
   </bookViews>
   <sheets>
     <sheet name="ANOVAs - percent dif" sheetId="1" r:id="rId1"/>
-    <sheet name="RCB ANOVAs - biomass" sheetId="4" r:id="rId2"/>
+    <sheet name="RCB ANOVAs" sheetId="4" r:id="rId2"/>
     <sheet name="ANOVAs - biomass by bioassay" sheetId="3" r:id="rId3"/>
     <sheet name="MANOVAs" sheetId="2" r:id="rId4"/>
   </sheets>
@@ -69,7 +69,7 @@
     <author>Catherine Schlenker</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{680926B3-4EF8-48D1-BD75-1E9C089DBA4E}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{69679FE7-5D23-4833-9C40-5CC337F6E170}">
       <text>
         <r>
           <rPr>
@@ -79,12 +79,21 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Catherine Schlenker:
-Independent variable for all = Treatment group</t>
+          <t>Catherine Schlenker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+R</t>
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{5A25EBA7-83F9-4DB7-8CA8-E0252739FFD7}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{4C4BEAB3-52EB-4CAA-BC58-295A3BAB25B7}">
       <text>
         <r>
           <rPr>
@@ -104,11 +113,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-using interaction between treatment and bioassay</t>
+R</t>
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{E198D16F-0D5A-4FB1-BBA7-302CADE3CA8C}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{6A357BA6-1B1E-4BAB-8691-84A5C7849192}">
       <text>
         <r>
           <rPr>
@@ -128,7 +137,32 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-using interaction between treatment and bioassay THIS IS FROM R</t>
+R
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{4BB63AE5-B8B0-4002-A5EF-5FE88D5BD7F0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Catherine Schlenker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+SPSS</t>
         </r>
       </text>
     </comment>
@@ -152,11 +186,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-using interaction between treatment and bioassay SPSS</t>
+SPSS</t>
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{B9F65478-D03E-459F-9CA6-7A32D119CB7A}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{D9EB1696-D184-4012-A634-D118005AA699}">
       <text>
         <r>
           <rPr>
@@ -176,12 +210,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-using interaction between treatment and bioassay SPSS
-</t>
+SPSS</t>
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{2DA4353C-DA3D-44AC-BCC0-A9038E4C7B94}">
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{872F2871-AAA1-4342-ACF5-FF650E7BA4AC}">
       <text>
         <r>
           <rPr>
@@ -191,12 +224,21 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Catherine Schlenker:
-Independent variable for all = Treatment group</t>
+          <t>Catherine Schlenker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+R</t>
         </r>
       </text>
     </comment>
-    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{7D1EBCDE-49C8-48B4-BF7D-6E9BC0D44771}">
+    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{A6118778-BF12-4458-A6D2-641E9A37C587}">
       <text>
         <r>
           <rPr>
@@ -206,12 +248,21 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Catherine Schlenker:
-Independent variable for all = Treatment group</t>
+          <t>Catherine Schlenker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+R</t>
         </r>
       </text>
     </comment>
-    <comment ref="A28" authorId="0" shapeId="0" xr:uid="{56CCD6C1-B988-457A-8624-39CD3F649224}">
+    <comment ref="J10" authorId="0" shapeId="0" xr:uid="{2ADC100C-A649-46F1-A97C-742847F74BFA}">
       <text>
         <r>
           <rPr>
@@ -221,8 +272,235 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Catherine Schlenker:
-Independent variable for all = Treatment group</t>
+          <t>Catherine Schlenker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+R
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K10" authorId="0" shapeId="0" xr:uid="{F28D20F7-039F-4811-9C6A-EA99D2F1DD55}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Catherine Schlenker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+SPSS</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L10" authorId="0" shapeId="0" xr:uid="{870CFC54-357F-447C-8B14-07B39FBDFA38}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Catherine Schlenker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+SPSS</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M10" authorId="0" shapeId="0" xr:uid="{F2D88C29-CE51-458A-A619-A1083C80E76E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Catherine Schlenker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+SPSS</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{D0AB5440-17CE-4933-BB8D-1357C534DCB7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Catherine Schlenker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+R</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I19" authorId="0" shapeId="0" xr:uid="{5646EB68-D454-4DD2-90CC-E44E1C8CDBFD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Catherine Schlenker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+R</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J19" authorId="0" shapeId="0" xr:uid="{A4262625-5642-48F9-B5DD-DFC912B6FF44}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Catherine Schlenker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+R
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K19" authorId="0" shapeId="0" xr:uid="{2E4D4C03-C8C4-4389-BC26-BF02C62C2017}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Catherine Schlenker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+SPSS</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L19" authorId="0" shapeId="0" xr:uid="{17512325-F837-44CF-9B82-100304F4B5B0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Catherine Schlenker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+SPSS</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M19" authorId="0" shapeId="0" xr:uid="{83BE35B5-31E4-4BEA-B892-445C1CBF4775}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Catherine Schlenker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+SPSS</t>
         </r>
       </text>
     </comment>
@@ -231,7 +509,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="160">
   <si>
     <t>Dependent variable (% change from control)</t>
   </si>
@@ -770,12 +1048,6 @@
     <t>df bioassay</t>
   </si>
   <si>
-    <t>f treatment</t>
-  </si>
-  <si>
-    <t>f bioassay</t>
-  </si>
-  <si>
     <t>p treatment</t>
   </si>
   <si>
@@ -791,9 +1063,6 @@
     <t>Dependent variable (ln(biomass))</t>
   </si>
   <si>
-    <t>Dependent variable (ln(percent change))</t>
-  </si>
-  <si>
     <t>Levene's test F</t>
   </si>
   <si>
@@ -803,7 +1072,25 @@
     <t>&lt;0.001</t>
   </si>
   <si>
-    <t>DF Levene;s</t>
+    <t>Main factor = Treatment, Block = Bioassay</t>
+  </si>
+  <si>
+    <t>F treatment</t>
+  </si>
+  <si>
+    <t>F bioassay</t>
+  </si>
+  <si>
+    <t>df Levene's</t>
+  </si>
+  <si>
+    <t>italics indicate slight difference in values between R and SPSS, usually only off by a few tenths</t>
+  </si>
+  <si>
+    <t>the RCB results (forst 6 columns) come from R</t>
+  </si>
+  <si>
+    <t>first three levene's results are from R, second 3 are SPSS</t>
   </si>
 </sst>
 </file>
@@ -922,7 +1209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -990,6 +1277,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1306,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A17F176-753C-47BC-A81F-3418BBE24096}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1599,11 +1887,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12773B5D-97E8-4039-B93C-89E44230DCC5}">
-  <dimension ref="A1:M1048576"/>
+  <dimension ref="A1:M1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D26" sqref="D26:G26"/>
+    <sheetView zoomScale="90" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1622,35 +1909,38 @@
       <c r="B1" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="F1" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="F1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G1" t="s">
-        <v>148</v>
-      </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="I1" t="s">
-        <v>153</v>
-      </c>
-      <c r="J1" t="s">
-        <v>154</v>
-      </c>
-      <c r="L1" t="s">
-        <v>153</v>
-      </c>
-      <c r="M1" t="s">
-        <v>154</v>
+      <c r="I1" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="K1" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -1670,7 +1960,7 @@
         <v>24.02</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G2" s="25">
         <v>1.9699999999999999E-12</v>
@@ -1691,7 +1981,7 @@
         <v>7.4809999999999999</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -1714,7 +2004,7 @@
         <v>1.2899999999999999E-3</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H3" s="30">
         <v>27</v>
@@ -1732,7 +2022,7 @@
         <v>4.5970000000000004</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1752,7 +2042,7 @@
         <v>14.18</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G4" s="34">
         <v>4.7199999999999999E-8</v>
@@ -1773,7 +2063,7 @@
         <v>22.89</v>
       </c>
       <c r="M4" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -1793,7 +2083,7 @@
         <v>19.68</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G5" s="34">
         <v>1.4000000000000001E-10</v>
@@ -1814,7 +2104,7 @@
         <v>6.5579999999999998</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -1834,7 +2124,7 @@
         <v>24.23</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G6" s="25">
         <v>1.61E-12</v>
@@ -1855,7 +2145,7 @@
         <v>6.391</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1896,7 +2186,7 @@
         <v>5.2960000000000003</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -1937,7 +2227,7 @@
         <v>3.2170000000000001</v>
       </c>
       <c r="M8" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1945,7 +2235,43 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="I10" s="22" t="s">
         <v>150</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="K10" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="M10" s="22" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -2113,25 +2439,43 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="F19" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="F19" t="s">
-        <v>147</v>
-      </c>
-      <c r="G19" t="s">
-        <v>148</v>
+      <c r="H19" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="I19" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="J19" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="K19" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="L19" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="M19" s="22" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -2151,10 +2495,10 @@
         <v>61.47</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H20" s="30">
         <v>27</v>
@@ -2172,7 +2516,7 @@
         <v>5.2130000000000001</v>
       </c>
       <c r="M20" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -2195,7 +2539,7 @@
         <v>1.64E-3</v>
       </c>
       <c r="G21" s="33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H21" s="30">
         <v>27</v>
@@ -2213,7 +2557,7 @@
         <v>5.1980000000000004</v>
       </c>
       <c r="M21" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -2233,7 +2577,7 @@
         <v>8.9459999999999997</v>
       </c>
       <c r="F22" s="33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G22" s="34">
         <v>1.9700000000000001E-5</v>
@@ -2254,7 +2598,7 @@
         <v>19.571000000000002</v>
       </c>
       <c r="M22" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -2274,7 +2618,7 @@
         <v>18.670000000000002</v>
       </c>
       <c r="F23" s="33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G23" s="34">
         <v>3.9399999999999998E-10</v>
@@ -2295,7 +2639,7 @@
         <v>6.2350000000000003</v>
       </c>
       <c r="M23" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -2315,10 +2659,10 @@
         <v>43.75</v>
       </c>
       <c r="F24" s="33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G24" s="33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H24" s="30">
         <v>27</v>
@@ -2336,7 +2680,7 @@
         <v>8.5640000000000001</v>
       </c>
       <c r="M24" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -2377,7 +2721,7 @@
         <v>4.6719999999999997</v>
       </c>
       <c r="M25" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -2418,180 +2762,56 @@
         <v>2.6989999999999998</v>
       </c>
       <c r="M26" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>152</v>
-      </c>
+      <c r="A28" s="1"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29">
-        <v>4</v>
-      </c>
-      <c r="C29">
-        <v>3</v>
-      </c>
-      <c r="D29">
-        <v>9.7650000000000006</v>
-      </c>
-      <c r="E29">
-        <v>3.355</v>
-      </c>
-      <c r="F29" s="24">
-        <v>9.4200000000000002E-4</v>
-      </c>
-      <c r="G29" s="23">
-        <v>5.5320000000000001E-2</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="F29" s="26"/>
+      <c r="G29" s="28"/>
       <c r="H29" s="28"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30">
-        <v>4</v>
-      </c>
-      <c r="C30">
-        <v>3</v>
-      </c>
-      <c r="D30">
-        <v>0.373</v>
-      </c>
-      <c r="E30">
-        <v>19.452000000000002</v>
-      </c>
-      <c r="F30">
-        <v>0.82299999999999995</v>
-      </c>
-      <c r="G30" s="25">
-        <v>6.6699999999999995E-5</v>
-      </c>
-      <c r="H30" s="28"/>
+        <v>158</v>
+      </c>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31">
-        <v>4</v>
-      </c>
-      <c r="C31">
-        <v>3</v>
-      </c>
-      <c r="D31">
-        <v>4.0810000000000004</v>
-      </c>
-      <c r="E31">
-        <v>4.4340000000000002</v>
-      </c>
-      <c r="F31" s="24">
-        <v>2.58E-2</v>
-      </c>
-      <c r="G31" s="24">
-        <v>2.5700000000000001E-2</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32">
-        <v>4</v>
-      </c>
-      <c r="C32">
-        <v>3</v>
-      </c>
-      <c r="D32">
-        <v>7.468</v>
-      </c>
-      <c r="E32">
-        <v>5.8280000000000003</v>
-      </c>
-      <c r="F32" s="24">
-        <v>2.9299999999999999E-3</v>
-      </c>
-      <c r="G32" s="24">
-        <v>1.0749999999999999E-2</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33">
-        <v>4</v>
-      </c>
-      <c r="C33">
-        <v>3</v>
-      </c>
-      <c r="D33">
-        <v>5.1920000000000002</v>
-      </c>
-      <c r="E33">
-        <v>4.8220000000000001</v>
-      </c>
-      <c r="F33" s="24">
-        <v>1.1599999999999999E-2</v>
-      </c>
-      <c r="G33" s="24">
-        <v>1.9900000000000001E-2</v>
-      </c>
+      <c r="A33" s="7"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34">
-        <v>4</v>
-      </c>
-      <c r="C34">
-        <v>3</v>
-      </c>
-      <c r="D34">
-        <v>1.548</v>
-      </c>
-      <c r="E34">
-        <v>6.5970000000000004</v>
-      </c>
-      <c r="F34" s="26">
-        <v>0.25048999999999999</v>
-      </c>
-      <c r="G34" s="24">
-        <v>6.9699999999999996E-3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35">
-        <v>4</v>
-      </c>
-      <c r="C35">
-        <v>3</v>
-      </c>
-      <c r="D35">
-        <v>0.90500000000000003</v>
-      </c>
-      <c r="E35">
-        <v>3.6640000000000001</v>
-      </c>
-      <c r="F35" s="26">
-        <v>0.49199999999999999</v>
-      </c>
-      <c r="G35" s="24">
-        <v>4.3999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="1048576" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M1048576" s="16" t="s">
-        <v>155</v>
+      <c r="A34" s="7"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+    </row>
+    <row r="1048575" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M1048575" s="16" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2605,7 +2825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02F6CD7-2B91-414A-B381-AE1014A5E445}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -2897,7 +3117,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>